<commit_message>
add mean model workflow.m automatic workflow.m creation update on tests
</commit_message>
<xml_diff>
--- a/src/code/templates/Output.xlsx
+++ b/src/code/templates/Output.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="240" windowWidth="19752" windowHeight="10992" activeTab="1"/>
+    <workbookView xWindow="192" yWindow="300" windowWidth="19752" windowHeight="9036" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="readme " sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="83">
   <si>
     <t>C_max</t>
   </si>
@@ -204,9 +204,6 @@
     <t>dataTpFilter</t>
   </si>
   <si>
-    <t>CodeIndtifier</t>
-  </si>
-  <si>
     <t>Output 1</t>
   </si>
   <si>
@@ -229,6 +226,45 @@
   </si>
   <si>
     <t>Code Identifier</t>
+  </si>
+  <si>
+    <t>residualScale</t>
+  </si>
+  <si>
+    <t>scale of residual, for lin residuals are calculated as data - simulation for log as log(data) - log(simulation)</t>
+  </si>
+  <si>
+    <t>log</t>
+  </si>
+  <si>
+    <t>lin</t>
+  </si>
+  <si>
+    <t>F_max</t>
+  </si>
+  <si>
+    <t>F_tEnd</t>
+  </si>
+  <si>
+    <t>F_max_t1_t2</t>
+  </si>
+  <si>
+    <t>F_max_tLast_tEnd</t>
+  </si>
+  <si>
+    <t>F_at_t2</t>
+  </si>
+  <si>
+    <t>F_at_tLast</t>
+  </si>
+  <si>
+    <t>PK Parameter calculated by default function. Attention the dimension has to be conserved</t>
+  </si>
+  <si>
+    <t>Output 3</t>
+  </si>
+  <si>
+    <t>Output 4</t>
   </si>
 </sst>
 </file>
@@ -254,7 +290,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -264,6 +300,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -280,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -293,6 +335,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -675,10 +727,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A7" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -689,21 +741,27 @@
     <col min="4" max="4" width="15.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>57</v>
       </c>
@@ -717,7 +775,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>58</v>
       </c>
@@ -731,12 +789,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" t="s">
         <v>39</v>
@@ -745,121 +803,117 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
         <v>68</v>
       </c>
-      <c r="C5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" s="5" t="s">
+      <c r="D12">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>11</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
@@ -868,40 +922,43 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C16" t="s">
         <v>4</v>
-      </c>
-      <c r="D14">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="D16">
         <v>-1</v>
@@ -912,10 +969,10 @@
         <v>60</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D17">
         <v>-1</v>
@@ -926,10 +983,7 @@
         <v>60</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D18">
         <v>-1</v>
@@ -940,13 +994,69 @@
         <v>60</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C21" t="s">
         <v>18</v>
       </c>
-      <c r="D19">
-        <v>-1</v>
+      <c r="D21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22">
+        <v>-1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23">
+        <v>-1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -957,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30:B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -968,25 +1078,31 @@
     <col min="2" max="2" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="E1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>42</v>
       </c>
       <c r="C2" t="s">
@@ -997,11 +1113,11 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="7" t="s">
         <v>38</v>
       </c>
       <c r="C3" t="s">
@@ -1011,12 +1127,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>67</v>
+      <c r="B4" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="C4" t="s">
         <v>39</v>
@@ -1025,48 +1141,44 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="69" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:6" ht="69" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="B5" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
       </c>
       <c r="C8" t="s">
         <v>39</v>
@@ -1075,12 +1187,12 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>1</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
@@ -1089,12 +1201,12 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="C10" t="s">
         <v>39</v>
@@ -1103,12 +1215,12 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
+    <row r="11" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -1117,40 +1229,40 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" t="s">
-        <v>25</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -1159,68 +1271,68 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C17" t="s">
         <v>39</v>
       </c>
-      <c r="D15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="D17">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C18" t="s">
         <v>39</v>
       </c>
-      <c r="D16">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="D18">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="C17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B18" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" t="s">
-        <v>30</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
@@ -1230,11 +1342,11 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" t="s">
-        <v>31</v>
+      <c r="A20" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
@@ -1244,11 +1356,11 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B21" t="s">
-        <v>32</v>
+      <c r="A21" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
@@ -1258,11 +1370,11 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B22" t="s">
-        <v>33</v>
+      <c r="A22" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
@@ -1272,11 +1384,11 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" t="s">
-        <v>34</v>
+      <c r="A23" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
@@ -1286,11 +1398,11 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B24" t="s">
-        <v>35</v>
+      <c r="A24" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
@@ -1300,39 +1412,39 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="A25" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="C25" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B26" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B27" t="s">
-        <v>36</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -1341,7 +1453,106 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30">
+        <v>-1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31">
+        <v>-1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32">
+        <v>-1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33">
+        <v>-1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34">
+        <v>-1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>